<commit_message>
Update test to match ID -> Id
</commit_message>
<xml_diff>
--- a/tests/testthat/test-excel-ui.xlsx
+++ b/tests/testthat/test-excel-ui.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr defaultThemeVersion="202300"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16965" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="14"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sections" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Inputs" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="GlobalPlotSettings" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="GlobalAxes_DDI_PredVsObs" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Lookup" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
   <si>
     <t>ID</t>
   </si>
@@ -557,7 +557,10 @@
     <t>GridLines</t>
   </si>
   <si>
-    <t xml:space="preserve">ID</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
   </si>
   <si>
     <t xml:space="preserve">Path</t>
@@ -698,7 +701,7 @@
     <t xml:space="preserve">FDA-ClinPharmReview_AI424-015_400mg_NormalSubjects</t>
   </si>
   <si>
-    <t xml:space="preserve">Observed Data</t>
+    <t xml:space="preserve">ObservedData</t>
   </si>
   <si>
     <t xml:space="preserve">Iwamoto 2008 - 800mg - Raltegravir - PO - 800 mg - Plasma - agg. (n=24)</t>
@@ -1115,7 +1118,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B3" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID"/>
+    <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Path"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1140,7 +1143,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Project"/>
     <tableColumn id="2" name="Simulation"/>
-    <tableColumn id="3" name="Observed Data"/>
+    <tableColumn id="3" name="ObservedData"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1150,7 +1153,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C4" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID"/>
+    <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="3" name="Type"/>
   </tableColumns>
@@ -1845,33 +1848,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2369,8 +2376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
@@ -2381,26 +2388,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2429,409 +2436,409 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
         <v>183</v>
-      </c>
-      <c r="C3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" t="s">
         <v>200</v>
-      </c>
-      <c r="C19" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C30" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C32" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C36" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2872,475 +2879,475 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C21" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C22" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C28" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C34" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C37" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C38" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C39" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C40" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C41" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C42" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C43" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3369,46 +3376,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
         <v>266</v>
-      </c>
-      <c r="B3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3449,1108 +3456,1108 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C14" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C18" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D18" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C19" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C20" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D21" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D33" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D34" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D35" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D36" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C37" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D37" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D38" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D39" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C40" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D40" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C41" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D41" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C42" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D42" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B43" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C43" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D43" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B44" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C44" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B45" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D45" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C47" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D47" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B48" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C48" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D48" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B49" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C49" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D49" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B50" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C50" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D50" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C51" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D51" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C52" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D52" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C53" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D53" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C54" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D54" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C55" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D55" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D56" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C57" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D57" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C58" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D58" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B59" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C59" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D59" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B60" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D60" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C61" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D61" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D62" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D63" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B64" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C64" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D64" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D65" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D66" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B67" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D67" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D68" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D69" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C70" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D70" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D71" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C72" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D73" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B74" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B75" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C75" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C76" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D76" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C77" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D77" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C78" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D78" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B79" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C79" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D79" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>